<commit_message>
Fix sum_up(). Update final Excel files.
</commit_message>
<xml_diff>
--- a/high school.xlsx
+++ b/high school.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$A$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$589</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -3683,10 +3683,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D589"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A578" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D577" sqref="D577"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A381" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A356" sqref="A356:D433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3707,7 +3709,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>8</v>
       </c>
@@ -3717,7 +3719,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>8</v>
       </c>
@@ -3727,7 +3729,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>8</v>
       </c>
@@ -3737,7 +3739,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>8</v>
       </c>
@@ -3747,7 +3749,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>8</v>
       </c>
@@ -3757,7 +3759,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>8</v>
       </c>
@@ -3767,7 +3769,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -3777,7 +3779,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3787,7 +3789,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -3797,7 +3799,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -3807,7 +3809,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -3817,7 +3819,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>8</v>
       </c>
@@ -3827,7 +3829,7 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>8</v>
       </c>
@@ -3837,7 +3839,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>8</v>
       </c>
@@ -3847,7 +3849,7 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>8</v>
       </c>
@@ -3857,7 +3859,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>8</v>
       </c>
@@ -3867,7 +3869,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>8</v>
       </c>
@@ -3877,7 +3879,7 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>8</v>
       </c>
@@ -3887,7 +3889,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>8</v>
       </c>
@@ -3897,7 +3899,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>8</v>
       </c>
@@ -3907,7 +3909,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>8</v>
       </c>
@@ -3917,7 +3919,7 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>8</v>
       </c>
@@ -3927,7 +3929,7 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>8</v>
       </c>
@@ -3937,7 +3939,7 @@
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>8</v>
       </c>
@@ -3947,7 +3949,7 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>8</v>
       </c>
@@ -3957,7 +3959,7 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>8</v>
       </c>
@@ -3967,7 +3969,7 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>8</v>
       </c>
@@ -3977,7 +3979,7 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>8</v>
       </c>
@@ -3987,7 +3989,7 @@
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>8</v>
       </c>
@@ -3997,7 +3999,7 @@
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>8</v>
       </c>
@@ -4007,7 +4009,7 @@
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>8</v>
       </c>
@@ -4017,7 +4019,7 @@
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <v>8</v>
       </c>
@@ -4027,7 +4029,7 @@
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <v>8</v>
       </c>
@@ -4037,7 +4039,7 @@
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <v>8</v>
       </c>
@@ -4047,7 +4049,7 @@
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>8</v>
       </c>
@@ -4057,7 +4059,7 @@
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <v>8</v>
       </c>
@@ -4067,7 +4069,7 @@
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <v>8</v>
       </c>
@@ -4077,7 +4079,7 @@
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>8</v>
       </c>
@@ -4087,7 +4089,7 @@
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>8</v>
       </c>
@@ -4097,7 +4099,7 @@
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>4</v>
       </c>
@@ -4107,7 +4109,7 @@
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3">
         <v>4</v>
       </c>
@@ -4117,7 +4119,7 @@
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3">
         <v>4</v>
       </c>
@@ -4127,7 +4129,7 @@
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3">
         <v>4</v>
       </c>
@@ -4137,7 +4139,7 @@
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3">
         <v>4</v>
       </c>
@@ -4147,7 +4149,7 @@
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3">
         <v>4</v>
       </c>
@@ -4157,7 +4159,7 @@
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3">
         <v>4</v>
       </c>
@@ -4167,7 +4169,7 @@
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3">
         <v>4</v>
       </c>
@@ -4177,7 +4179,7 @@
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A49" s="3">
         <v>4</v>
       </c>
@@ -4187,7 +4189,7 @@
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A50" s="3">
         <v>4</v>
       </c>
@@ -4197,7 +4199,7 @@
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A51" s="3">
         <v>4</v>
       </c>
@@ -4207,7 +4209,7 @@
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A52" s="3">
         <v>4</v>
       </c>
@@ -4217,7 +4219,7 @@
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A53" s="3">
         <v>4</v>
       </c>
@@ -4227,7 +4229,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A54" s="3">
         <v>4</v>
       </c>
@@ -4237,7 +4239,7 @@
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A55" s="3">
         <v>4</v>
       </c>
@@ -4247,7 +4249,7 @@
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A56" s="3">
         <v>4</v>
       </c>
@@ -4257,7 +4259,7 @@
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3">
         <v>4</v>
       </c>
@@ -4267,7 +4269,7 @@
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A58" s="3">
         <v>4</v>
       </c>
@@ -4277,7 +4279,7 @@
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A59" s="3">
         <v>4</v>
       </c>
@@ -4287,7 +4289,7 @@
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A60" s="3">
         <v>4</v>
       </c>
@@ -4297,7 +4299,7 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3">
         <v>4</v>
       </c>
@@ -4307,7 +4309,7 @@
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A62" s="3">
         <v>4</v>
       </c>
@@ -4317,7 +4319,7 @@
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A63" s="3">
         <v>4</v>
       </c>
@@ -4327,7 +4329,7 @@
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A64" s="3">
         <v>4</v>
       </c>
@@ -4337,7 +4339,7 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
     </row>
-    <row r="65" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A65" s="3">
         <v>4</v>
       </c>
@@ -4347,7 +4349,7 @@
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A66" s="3">
         <v>4</v>
       </c>
@@ -4357,7 +4359,7 @@
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
     </row>
-    <row r="67" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A67" s="3">
         <v>4</v>
       </c>
@@ -4367,7 +4369,7 @@
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
     </row>
-    <row r="68" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A68" s="3">
         <v>4</v>
       </c>
@@ -4377,7 +4379,7 @@
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
     </row>
-    <row r="69" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A69" s="3">
         <v>4</v>
       </c>
@@ -4387,7 +4389,7 @@
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
     </row>
-    <row r="70" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A70" s="3">
         <v>4</v>
       </c>
@@ -4397,7 +4399,7 @@
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
     </row>
-    <row r="71" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A71" s="3">
         <v>4</v>
       </c>
@@ -4407,7 +4409,7 @@
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
     </row>
-    <row r="72" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A72" s="3">
         <v>4</v>
       </c>
@@ -4417,7 +4419,7 @@
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
     </row>
-    <row r="73" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A73" s="3">
         <v>4</v>
       </c>
@@ -4427,7 +4429,7 @@
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A74" s="3">
         <v>4</v>
       </c>
@@ -4437,7 +4439,7 @@
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
     </row>
-    <row r="75" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A75" s="3">
         <v>4</v>
       </c>
@@ -4447,7 +4449,7 @@
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
     </row>
-    <row r="76" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A76" s="3">
         <v>4</v>
       </c>
@@ -4457,7 +4459,7 @@
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A77" s="3">
         <v>4</v>
       </c>
@@ -4467,7 +4469,7 @@
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
     </row>
-    <row r="78" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A78" s="3">
         <v>4</v>
       </c>
@@ -4477,7 +4479,7 @@
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A79" s="3">
         <v>4</v>
       </c>
@@ -4487,7 +4489,7 @@
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
     </row>
-    <row r="80" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A80" s="3">
         <v>5</v>
       </c>
@@ -4497,7 +4499,7 @@
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
     </row>
-    <row r="81" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A81" s="3">
         <v>5</v>
       </c>
@@ -4507,7 +4509,7 @@
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
     </row>
-    <row r="82" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A82" s="3">
         <v>5</v>
       </c>
@@ -4517,7 +4519,7 @@
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
     </row>
-    <row r="83" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A83" s="3">
         <v>5</v>
       </c>
@@ -4527,7 +4529,7 @@
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A84" s="3">
         <v>5</v>
       </c>
@@ -4537,7 +4539,7 @@
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
     </row>
-    <row r="85" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A85" s="3">
         <v>5</v>
       </c>
@@ -4547,7 +4549,7 @@
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
     </row>
-    <row r="86" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A86" s="3">
         <v>5</v>
       </c>
@@ -4557,7 +4559,7 @@
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
     </row>
-    <row r="87" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A87" s="3">
         <v>5</v>
       </c>
@@ -4567,7 +4569,7 @@
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A88" s="3">
         <v>5</v>
       </c>
@@ -4577,7 +4579,7 @@
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
     </row>
-    <row r="89" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A89" s="3">
         <v>5</v>
       </c>
@@ -4587,7 +4589,7 @@
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
     </row>
-    <row r="90" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A90" s="3">
         <v>5</v>
       </c>
@@ -4597,7 +4599,7 @@
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
     </row>
-    <row r="91" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A91" s="3">
         <v>5</v>
       </c>
@@ -4607,7 +4609,7 @@
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
     </row>
-    <row r="92" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A92" s="3">
         <v>5</v>
       </c>
@@ -4617,7 +4619,7 @@
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
     </row>
-    <row r="93" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A93" s="3">
         <v>5</v>
       </c>
@@ -4627,7 +4629,7 @@
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
     </row>
-    <row r="94" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A94" s="3">
         <v>5</v>
       </c>
@@ -4637,7 +4639,7 @@
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
     </row>
-    <row r="95" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A95" s="3">
         <v>5</v>
       </c>
@@ -4647,7 +4649,7 @@
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
     </row>
-    <row r="96" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A96" s="3">
         <v>5</v>
       </c>
@@ -4657,7 +4659,7 @@
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
     </row>
-    <row r="97" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A97" s="3">
         <v>5</v>
       </c>
@@ -4667,7 +4669,7 @@
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
     </row>
-    <row r="98" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A98" s="3">
         <v>5</v>
       </c>
@@ -4677,7 +4679,7 @@
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
     </row>
-    <row r="99" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A99" s="3">
         <v>5</v>
       </c>
@@ -4687,7 +4689,7 @@
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
     </row>
-    <row r="100" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A100" s="3">
         <v>5</v>
       </c>
@@ -4697,7 +4699,7 @@
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
     </row>
-    <row r="101" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A101" s="3">
         <v>5</v>
       </c>
@@ -4707,7 +4709,7 @@
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
     </row>
-    <row r="102" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A102" s="3">
         <v>5</v>
       </c>
@@ -4717,7 +4719,7 @@
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
     </row>
-    <row r="103" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A103" s="3">
         <v>5</v>
       </c>
@@ -4727,7 +4729,7 @@
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
     </row>
-    <row r="104" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A104" s="3">
         <v>5</v>
       </c>
@@ -4737,7 +4739,7 @@
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
     </row>
-    <row r="105" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A105" s="3">
         <v>5</v>
       </c>
@@ -4747,7 +4749,7 @@
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
     </row>
-    <row r="106" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A106" s="3">
         <v>5</v>
       </c>
@@ -4757,7 +4759,7 @@
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
     </row>
-    <row r="107" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A107" s="3">
         <v>5</v>
       </c>
@@ -4767,7 +4769,7 @@
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
     </row>
-    <row r="108" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A108" s="3">
         <v>5</v>
       </c>
@@ -4777,7 +4779,7 @@
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
     </row>
-    <row r="109" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A109" s="3">
         <v>5</v>
       </c>
@@ -4787,7 +4789,7 @@
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
     </row>
-    <row r="110" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A110" s="3">
         <v>5</v>
       </c>
@@ -4797,7 +4799,7 @@
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
     </row>
-    <row r="111" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A111" s="3">
         <v>5</v>
       </c>
@@ -4807,7 +4809,7 @@
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
     </row>
-    <row r="112" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A112" s="3">
         <v>5</v>
       </c>
@@ -4817,7 +4819,7 @@
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
     </row>
-    <row r="113" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A113" s="3">
         <v>5</v>
       </c>
@@ -4827,7 +4829,7 @@
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
     </row>
-    <row r="114" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A114" s="3">
         <v>5</v>
       </c>
@@ -4837,7 +4839,7 @@
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
     </row>
-    <row r="115" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A115" s="3">
         <v>5</v>
       </c>
@@ -4847,7 +4849,7 @@
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
     </row>
-    <row r="116" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A116" s="3">
         <v>5</v>
       </c>
@@ -4857,7 +4859,7 @@
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
     </row>
-    <row r="117" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A117" s="3">
         <v>5</v>
       </c>
@@ -4867,7 +4869,7 @@
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
     </row>
-    <row r="118" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A118" s="3">
         <v>5</v>
       </c>
@@ -4877,7 +4879,7 @@
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
     </row>
-    <row r="119" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A119" s="3">
         <v>1</v>
       </c>
@@ -4889,7 +4891,7 @@
       </c>
       <c r="D119" s="4"/>
     </row>
-    <row r="120" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A120" s="3">
         <v>1</v>
       </c>
@@ -4901,7 +4903,7 @@
       </c>
       <c r="D120" s="4"/>
     </row>
-    <row r="121" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A121" s="3">
         <v>1</v>
       </c>
@@ -4913,7 +4915,7 @@
       </c>
       <c r="D121" s="4"/>
     </row>
-    <row r="122" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A122" s="3">
         <v>1</v>
       </c>
@@ -4925,7 +4927,7 @@
       </c>
       <c r="D122" s="4"/>
     </row>
-    <row r="123" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A123" s="3">
         <v>1</v>
       </c>
@@ -4937,7 +4939,7 @@
       </c>
       <c r="D123" s="4"/>
     </row>
-    <row r="124" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A124" s="3">
         <v>1</v>
       </c>
@@ -4949,7 +4951,7 @@
       </c>
       <c r="D124" s="4"/>
     </row>
-    <row r="125" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A125" s="3">
         <v>1</v>
       </c>
@@ -4961,7 +4963,7 @@
       </c>
       <c r="D125" s="4"/>
     </row>
-    <row r="126" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A126" s="3">
         <v>1</v>
       </c>
@@ -4973,7 +4975,7 @@
       </c>
       <c r="D126" s="4"/>
     </row>
-    <row r="127" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A127" s="3">
         <v>1</v>
       </c>
@@ -4985,7 +4987,7 @@
       </c>
       <c r="D127" s="4"/>
     </row>
-    <row r="128" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A128" s="3">
         <v>1</v>
       </c>
@@ -4997,7 +4999,7 @@
       </c>
       <c r="D128" s="4"/>
     </row>
-    <row r="129" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A129" s="3">
         <v>1</v>
       </c>
@@ -5009,7 +5011,7 @@
       </c>
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A130" s="3">
         <v>1</v>
       </c>
@@ -5021,7 +5023,7 @@
       </c>
       <c r="D130" s="4"/>
     </row>
-    <row r="131" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A131" s="3">
         <v>1</v>
       </c>
@@ -5033,7 +5035,7 @@
       </c>
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A132" s="3">
         <v>1</v>
       </c>
@@ -5045,7 +5047,7 @@
       </c>
       <c r="D132" s="4"/>
     </row>
-    <row r="133" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A133" s="3">
         <v>1</v>
       </c>
@@ -5057,7 +5059,7 @@
       </c>
       <c r="D133" s="4"/>
     </row>
-    <row r="134" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A134" s="3">
         <v>1</v>
       </c>
@@ -5069,7 +5071,7 @@
       </c>
       <c r="D134" s="4"/>
     </row>
-    <row r="135" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A135" s="3">
         <v>1</v>
       </c>
@@ -5081,7 +5083,7 @@
       </c>
       <c r="D135" s="4"/>
     </row>
-    <row r="136" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A136" s="3">
         <v>1</v>
       </c>
@@ -5093,7 +5095,7 @@
       </c>
       <c r="D136" s="4"/>
     </row>
-    <row r="137" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A137" s="3">
         <v>1</v>
       </c>
@@ -5105,7 +5107,7 @@
       </c>
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A138" s="3">
         <v>1</v>
       </c>
@@ -5117,7 +5119,7 @@
       </c>
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A139" s="3">
         <v>1</v>
       </c>
@@ -5129,7 +5131,7 @@
       </c>
       <c r="D139" s="4"/>
     </row>
-    <row r="140" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A140" s="3">
         <v>1</v>
       </c>
@@ -5141,7 +5143,7 @@
       </c>
       <c r="D140" s="4"/>
     </row>
-    <row r="141" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A141" s="3">
         <v>1</v>
       </c>
@@ -5153,7 +5155,7 @@
       </c>
       <c r="D141" s="4"/>
     </row>
-    <row r="142" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A142" s="3">
         <v>1</v>
       </c>
@@ -5165,7 +5167,7 @@
       </c>
       <c r="D142" s="4"/>
     </row>
-    <row r="143" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A143" s="3">
         <v>1</v>
       </c>
@@ -5177,7 +5179,7 @@
       </c>
       <c r="D143" s="4"/>
     </row>
-    <row r="144" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A144" s="3">
         <v>1</v>
       </c>
@@ -5189,7 +5191,7 @@
       </c>
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A145" s="3">
         <v>1</v>
       </c>
@@ -5201,7 +5203,7 @@
       </c>
       <c r="D145" s="4"/>
     </row>
-    <row r="146" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A146" s="3">
         <v>1</v>
       </c>
@@ -5213,7 +5215,7 @@
       </c>
       <c r="D146" s="4"/>
     </row>
-    <row r="147" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A147" s="3">
         <v>1</v>
       </c>
@@ -5225,7 +5227,7 @@
       </c>
       <c r="D147" s="4"/>
     </row>
-    <row r="148" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A148" s="3">
         <v>1</v>
       </c>
@@ -5237,7 +5239,7 @@
       </c>
       <c r="D148" s="4"/>
     </row>
-    <row r="149" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A149" s="3">
         <v>1</v>
       </c>
@@ -5249,7 +5251,7 @@
       </c>
       <c r="D149" s="4"/>
     </row>
-    <row r="150" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A150" s="3">
         <v>1</v>
       </c>
@@ -5261,7 +5263,7 @@
       </c>
       <c r="D150" s="4"/>
     </row>
-    <row r="151" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A151" s="3">
         <v>1</v>
       </c>
@@ -5273,7 +5275,7 @@
       </c>
       <c r="D151" s="4"/>
     </row>
-    <row r="152" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A152" s="3">
         <v>1</v>
       </c>
@@ -5285,7 +5287,7 @@
       </c>
       <c r="D152" s="4"/>
     </row>
-    <row r="153" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A153" s="3">
         <v>1</v>
       </c>
@@ -5297,7 +5299,7 @@
       </c>
       <c r="D153" s="4"/>
     </row>
-    <row r="154" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A154" s="3">
         <v>1</v>
       </c>
@@ -5309,7 +5311,7 @@
       </c>
       <c r="D154" s="4"/>
     </row>
-    <row r="155" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A155" s="3">
         <v>1</v>
       </c>
@@ -5321,7 +5323,7 @@
       </c>
       <c r="D155" s="4"/>
     </row>
-    <row r="156" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A156" s="3">
         <v>1</v>
       </c>
@@ -5333,7 +5335,7 @@
       </c>
       <c r="D156" s="4"/>
     </row>
-    <row r="157" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A157" s="3">
         <v>1</v>
       </c>
@@ -5345,7 +5347,7 @@
       </c>
       <c r="D157" s="4"/>
     </row>
-    <row r="158" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A158" s="3">
         <v>1</v>
       </c>
@@ -5357,7 +5359,7 @@
       </c>
       <c r="D158" s="4"/>
     </row>
-    <row r="159" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A159" s="3">
         <v>2</v>
       </c>
@@ -5369,7 +5371,7 @@
       </c>
       <c r="D159" s="4"/>
     </row>
-    <row r="160" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A160" s="3">
         <v>2</v>
       </c>
@@ -5381,7 +5383,7 @@
       </c>
       <c r="D160" s="4"/>
     </row>
-    <row r="161" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A161" s="3">
         <v>2</v>
       </c>
@@ -5393,7 +5395,7 @@
       </c>
       <c r="D161" s="4"/>
     </row>
-    <row r="162" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A162" s="3">
         <v>2</v>
       </c>
@@ -5405,7 +5407,7 @@
       </c>
       <c r="D162" s="4"/>
     </row>
-    <row r="163" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A163" s="3">
         <v>2</v>
       </c>
@@ -5417,7 +5419,7 @@
       </c>
       <c r="D163" s="4"/>
     </row>
-    <row r="164" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A164" s="3">
         <v>2</v>
       </c>
@@ -5429,7 +5431,7 @@
       </c>
       <c r="D164" s="4"/>
     </row>
-    <row r="165" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A165" s="3">
         <v>2</v>
       </c>
@@ -5443,7 +5445,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A166" s="3">
         <v>2</v>
       </c>
@@ -5451,7 +5453,7 @@
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
     </row>
-    <row r="167" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A167" s="3">
         <v>2</v>
       </c>
@@ -5463,7 +5465,7 @@
       </c>
       <c r="D167" s="4"/>
     </row>
-    <row r="168" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A168" s="3">
         <v>2</v>
       </c>
@@ -5475,7 +5477,7 @@
       </c>
       <c r="D168" s="4"/>
     </row>
-    <row r="169" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A169" s="3">
         <v>2</v>
       </c>
@@ -5487,7 +5489,7 @@
       </c>
       <c r="D169" s="4"/>
     </row>
-    <row r="170" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A170" s="3">
         <v>2</v>
       </c>
@@ -5499,7 +5501,7 @@
       </c>
       <c r="D170" s="4"/>
     </row>
-    <row r="171" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A171" s="3">
         <v>2</v>
       </c>
@@ -5511,7 +5513,7 @@
       </c>
       <c r="D171" s="4"/>
     </row>
-    <row r="172" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A172" s="3">
         <v>2</v>
       </c>
@@ -5523,7 +5525,7 @@
       </c>
       <c r="D172" s="4"/>
     </row>
-    <row r="173" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A173" s="3">
         <v>2</v>
       </c>
@@ -5535,7 +5537,7 @@
       </c>
       <c r="D173" s="4"/>
     </row>
-    <row r="174" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A174" s="3">
         <v>2</v>
       </c>
@@ -5547,7 +5549,7 @@
       </c>
       <c r="D174" s="4"/>
     </row>
-    <row r="175" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A175" s="3">
         <v>2</v>
       </c>
@@ -5559,7 +5561,7 @@
       </c>
       <c r="D175" s="4"/>
     </row>
-    <row r="176" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A176" s="3">
         <v>2</v>
       </c>
@@ -5571,7 +5573,7 @@
       </c>
       <c r="D176" s="4"/>
     </row>
-    <row r="177" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A177" s="3">
         <v>2</v>
       </c>
@@ -5583,7 +5585,7 @@
       </c>
       <c r="D177" s="4"/>
     </row>
-    <row r="178" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A178" s="3">
         <v>2</v>
       </c>
@@ -5595,7 +5597,7 @@
       </c>
       <c r="D178" s="4"/>
     </row>
-    <row r="179" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A179" s="3">
         <v>2</v>
       </c>
@@ -5607,7 +5609,7 @@
       </c>
       <c r="D179" s="4"/>
     </row>
-    <row r="180" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A180" s="3">
         <v>2</v>
       </c>
@@ -5619,7 +5621,7 @@
       </c>
       <c r="D180" s="4"/>
     </row>
-    <row r="181" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A181" s="3">
         <v>2</v>
       </c>
@@ -5633,7 +5635,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A182" s="3">
         <v>2</v>
       </c>
@@ -5645,7 +5647,7 @@
       </c>
       <c r="D182" s="4"/>
     </row>
-    <row r="183" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A183" s="3">
         <v>2</v>
       </c>
@@ -5657,7 +5659,7 @@
       </c>
       <c r="D183" s="4"/>
     </row>
-    <row r="184" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A184" s="3">
         <v>2</v>
       </c>
@@ -5669,7 +5671,7 @@
       </c>
       <c r="D184" s="4"/>
     </row>
-    <row r="185" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A185" s="3">
         <v>2</v>
       </c>
@@ -5681,7 +5683,7 @@
       </c>
       <c r="D185" s="4"/>
     </row>
-    <row r="186" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A186" s="3">
         <v>2</v>
       </c>
@@ -5693,7 +5695,7 @@
       </c>
       <c r="D186" s="4"/>
     </row>
-    <row r="187" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A187" s="3">
         <v>2</v>
       </c>
@@ -5705,7 +5707,7 @@
       </c>
       <c r="D187" s="4"/>
     </row>
-    <row r="188" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A188" s="3">
         <v>2</v>
       </c>
@@ -5717,7 +5719,7 @@
       </c>
       <c r="D188" s="4"/>
     </row>
-    <row r="189" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A189" s="3">
         <v>2</v>
       </c>
@@ -5729,7 +5731,7 @@
       </c>
       <c r="D189" s="4"/>
     </row>
-    <row r="190" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A190" s="3">
         <v>2</v>
       </c>
@@ -5741,7 +5743,7 @@
       </c>
       <c r="D190" s="4"/>
     </row>
-    <row r="191" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A191" s="3">
         <v>2</v>
       </c>
@@ -5753,7 +5755,7 @@
       </c>
       <c r="D191" s="4"/>
     </row>
-    <row r="192" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A192" s="3">
         <v>2</v>
       </c>
@@ -5765,7 +5767,7 @@
       </c>
       <c r="D192" s="4"/>
     </row>
-    <row r="193" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A193" s="3">
         <v>2</v>
       </c>
@@ -5777,7 +5779,7 @@
       </c>
       <c r="D193" s="4"/>
     </row>
-    <row r="194" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A194" s="3">
         <v>2</v>
       </c>
@@ -5789,7 +5791,7 @@
       </c>
       <c r="D194" s="4"/>
     </row>
-    <row r="195" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A195" s="3">
         <v>2</v>
       </c>
@@ -5801,7 +5803,7 @@
       </c>
       <c r="D195" s="4"/>
     </row>
-    <row r="196" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A196" s="3">
         <v>2</v>
       </c>
@@ -5813,7 +5815,7 @@
       </c>
       <c r="D196" s="4"/>
     </row>
-    <row r="197" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A197" s="3">
         <v>2</v>
       </c>
@@ -5825,7 +5827,7 @@
       </c>
       <c r="D197" s="4"/>
     </row>
-    <row r="198" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A198" s="3">
         <v>2</v>
       </c>
@@ -5837,7 +5839,7 @@
       </c>
       <c r="D198" s="4"/>
     </row>
-    <row r="199" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A199" s="3">
         <v>3</v>
       </c>
@@ -5849,7 +5851,7 @@
       </c>
       <c r="D199" s="4"/>
     </row>
-    <row r="200" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A200" s="3">
         <v>3</v>
       </c>
@@ -5861,7 +5863,7 @@
       </c>
       <c r="D200" s="4"/>
     </row>
-    <row r="201" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A201" s="3">
         <v>3</v>
       </c>
@@ -5873,7 +5875,7 @@
       </c>
       <c r="D201" s="4"/>
     </row>
-    <row r="202" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A202" s="3">
         <v>3</v>
       </c>
@@ -5887,7 +5889,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A203" s="3">
         <v>3</v>
       </c>
@@ -5899,7 +5901,7 @@
       </c>
       <c r="D203" s="4"/>
     </row>
-    <row r="204" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A204" s="3">
         <v>3</v>
       </c>
@@ -5911,7 +5913,7 @@
       </c>
       <c r="D204" s="4"/>
     </row>
-    <row r="205" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A205" s="3">
         <v>3</v>
       </c>
@@ -5923,7 +5925,7 @@
       </c>
       <c r="D205" s="4"/>
     </row>
-    <row r="206" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A206" s="3">
         <v>3</v>
       </c>
@@ -5935,7 +5937,7 @@
       </c>
       <c r="D206" s="4"/>
     </row>
-    <row r="207" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A207" s="3">
         <v>3</v>
       </c>
@@ -5947,7 +5949,7 @@
       </c>
       <c r="D207" s="4"/>
     </row>
-    <row r="208" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A208" s="3">
         <v>3</v>
       </c>
@@ -5959,7 +5961,7 @@
       </c>
       <c r="D208" s="4"/>
     </row>
-    <row r="209" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A209" s="3">
         <v>3</v>
       </c>
@@ -5971,7 +5973,7 @@
       </c>
       <c r="D209" s="4"/>
     </row>
-    <row r="210" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A210" s="3">
         <v>3</v>
       </c>
@@ -5983,7 +5985,7 @@
       </c>
       <c r="D210" s="4"/>
     </row>
-    <row r="211" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A211" s="3">
         <v>3</v>
       </c>
@@ -5995,7 +5997,7 @@
       </c>
       <c r="D211" s="4"/>
     </row>
-    <row r="212" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A212" s="3">
         <v>3</v>
       </c>
@@ -6007,7 +6009,7 @@
       </c>
       <c r="D212" s="4"/>
     </row>
-    <row r="213" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A213" s="3">
         <v>3</v>
       </c>
@@ -6019,7 +6021,7 @@
       </c>
       <c r="D213" s="4"/>
     </row>
-    <row r="214" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A214" s="3">
         <v>3</v>
       </c>
@@ -6031,7 +6033,7 @@
       </c>
       <c r="D214" s="4"/>
     </row>
-    <row r="215" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A215" s="3">
         <v>3</v>
       </c>
@@ -6043,7 +6045,7 @@
       </c>
       <c r="D215" s="4"/>
     </row>
-    <row r="216" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A216" s="3">
         <v>3</v>
       </c>
@@ -6055,7 +6057,7 @@
       </c>
       <c r="D216" s="4"/>
     </row>
-    <row r="217" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A217" s="3">
         <v>3</v>
       </c>
@@ -6067,7 +6069,7 @@
       </c>
       <c r="D217" s="4"/>
     </row>
-    <row r="218" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A218" s="3">
         <v>3</v>
       </c>
@@ -6079,7 +6081,7 @@
       </c>
       <c r="D218" s="4"/>
     </row>
-    <row r="219" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A219" s="3">
         <v>3</v>
       </c>
@@ -6091,7 +6093,7 @@
       </c>
       <c r="D219" s="4"/>
     </row>
-    <row r="220" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A220" s="3">
         <v>3</v>
       </c>
@@ -6103,7 +6105,7 @@
       </c>
       <c r="D220" s="4"/>
     </row>
-    <row r="221" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A221" s="3">
         <v>3</v>
       </c>
@@ -6115,7 +6117,7 @@
       </c>
       <c r="D221" s="4"/>
     </row>
-    <row r="222" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A222" s="3">
         <v>3</v>
       </c>
@@ -6127,7 +6129,7 @@
       </c>
       <c r="D222" s="4"/>
     </row>
-    <row r="223" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A223" s="3">
         <v>3</v>
       </c>
@@ -6139,7 +6141,7 @@
       </c>
       <c r="D223" s="4"/>
     </row>
-    <row r="224" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A224" s="3">
         <v>3</v>
       </c>
@@ -6151,7 +6153,7 @@
       </c>
       <c r="D224" s="4"/>
     </row>
-    <row r="225" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A225" s="3">
         <v>3</v>
       </c>
@@ -6163,7 +6165,7 @@
       </c>
       <c r="D225" s="4"/>
     </row>
-    <row r="226" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A226" s="3">
         <v>3</v>
       </c>
@@ -6175,7 +6177,7 @@
       </c>
       <c r="D226" s="4"/>
     </row>
-    <row r="227" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A227" s="3">
         <v>3</v>
       </c>
@@ -6187,7 +6189,7 @@
       </c>
       <c r="D227" s="4"/>
     </row>
-    <row r="228" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A228" s="3">
         <v>3</v>
       </c>
@@ -6199,7 +6201,7 @@
       </c>
       <c r="D228" s="4"/>
     </row>
-    <row r="229" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A229" s="3">
         <v>3</v>
       </c>
@@ -6211,7 +6213,7 @@
       </c>
       <c r="D229" s="4"/>
     </row>
-    <row r="230" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A230" s="3">
         <v>3</v>
       </c>
@@ -6223,7 +6225,7 @@
       </c>
       <c r="D230" s="4"/>
     </row>
-    <row r="231" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A231" s="3">
         <v>3</v>
       </c>
@@ -6235,7 +6237,7 @@
       </c>
       <c r="D231" s="4"/>
     </row>
-    <row r="232" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A232" s="3">
         <v>3</v>
       </c>
@@ -6247,7 +6249,7 @@
       </c>
       <c r="D232" s="4"/>
     </row>
-    <row r="233" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A233" s="3">
         <v>3</v>
       </c>
@@ -6259,7 +6261,7 @@
       </c>
       <c r="D233" s="4"/>
     </row>
-    <row r="234" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A234" s="3">
         <v>3</v>
       </c>
@@ -6271,7 +6273,7 @@
       </c>
       <c r="D234" s="4"/>
     </row>
-    <row r="235" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A235" s="3">
         <v>3</v>
       </c>
@@ -6283,7 +6285,7 @@
       </c>
       <c r="D235" s="4"/>
     </row>
-    <row r="236" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A236" s="3">
         <v>3</v>
       </c>
@@ -6295,7 +6297,7 @@
       </c>
       <c r="D236" s="4"/>
     </row>
-    <row r="237" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A237" s="3">
         <v>3</v>
       </c>
@@ -6307,7 +6309,7 @@
       </c>
       <c r="D237" s="4"/>
     </row>
-    <row r="238" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A238" s="3">
         <v>3</v>
       </c>
@@ -6319,7 +6321,7 @@
       </c>
       <c r="D238" s="4"/>
     </row>
-    <row r="239" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A239" s="3">
         <v>6</v>
       </c>
@@ -6331,7 +6333,7 @@
       </c>
       <c r="D239" s="4"/>
     </row>
-    <row r="240" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A240" s="3">
         <v>6</v>
       </c>
@@ -6343,7 +6345,7 @@
       </c>
       <c r="D240" s="4"/>
     </row>
-    <row r="241" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A241" s="3">
         <v>6</v>
       </c>
@@ -6355,7 +6357,7 @@
       </c>
       <c r="D241" s="4"/>
     </row>
-    <row r="242" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A242" s="3">
         <v>6</v>
       </c>
@@ -6367,7 +6369,7 @@
       </c>
       <c r="D242" s="4"/>
     </row>
-    <row r="243" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A243" s="3">
         <v>6</v>
       </c>
@@ -6379,7 +6381,7 @@
       </c>
       <c r="D243" s="4"/>
     </row>
-    <row r="244" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A244" s="3">
         <v>6</v>
       </c>
@@ -6391,7 +6393,7 @@
       </c>
       <c r="D244" s="4"/>
     </row>
-    <row r="245" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A245" s="3">
         <v>6</v>
       </c>
@@ -6403,7 +6405,7 @@
       </c>
       <c r="D245" s="4"/>
     </row>
-    <row r="246" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A246" s="3">
         <v>6</v>
       </c>
@@ -6415,7 +6417,7 @@
       </c>
       <c r="D246" s="4"/>
     </row>
-    <row r="247" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A247" s="3">
         <v>6</v>
       </c>
@@ -6427,7 +6429,7 @@
       </c>
       <c r="D247" s="4"/>
     </row>
-    <row r="248" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A248" s="3">
         <v>6</v>
       </c>
@@ -6439,7 +6441,7 @@
       </c>
       <c r="D248" s="4"/>
     </row>
-    <row r="249" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A249" s="3">
         <v>6</v>
       </c>
@@ -6451,7 +6453,7 @@
       </c>
       <c r="D249" s="4"/>
     </row>
-    <row r="250" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A250" s="3">
         <v>6</v>
       </c>
@@ -6463,7 +6465,7 @@
       </c>
       <c r="D250" s="4"/>
     </row>
-    <row r="251" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A251" s="3">
         <v>6</v>
       </c>
@@ -6475,7 +6477,7 @@
       </c>
       <c r="D251" s="4"/>
     </row>
-    <row r="252" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A252" s="3">
         <v>6</v>
       </c>
@@ -6487,7 +6489,7 @@
       </c>
       <c r="D252" s="4"/>
     </row>
-    <row r="253" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A253" s="3">
         <v>6</v>
       </c>
@@ -6499,7 +6501,7 @@
       </c>
       <c r="D253" s="4"/>
     </row>
-    <row r="254" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A254" s="3">
         <v>6</v>
       </c>
@@ -6511,7 +6513,7 @@
       </c>
       <c r="D254" s="4"/>
     </row>
-    <row r="255" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A255" s="3">
         <v>6</v>
       </c>
@@ -6523,7 +6525,7 @@
       </c>
       <c r="D255" s="4"/>
     </row>
-    <row r="256" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A256" s="3">
         <v>6</v>
       </c>
@@ -6535,7 +6537,7 @@
       </c>
       <c r="D256" s="4"/>
     </row>
-    <row r="257" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A257" s="3">
         <v>6</v>
       </c>
@@ -6547,7 +6549,7 @@
       </c>
       <c r="D257" s="4"/>
     </row>
-    <row r="258" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A258" s="3">
         <v>6</v>
       </c>
@@ -6559,7 +6561,7 @@
       </c>
       <c r="D258" s="4"/>
     </row>
-    <row r="259" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A259" s="3">
         <v>6</v>
       </c>
@@ -6571,7 +6573,7 @@
       </c>
       <c r="D259" s="4"/>
     </row>
-    <row r="260" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A260" s="3">
         <v>6</v>
       </c>
@@ -6583,7 +6585,7 @@
       </c>
       <c r="D260" s="4"/>
     </row>
-    <row r="261" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A261" s="3">
         <v>6</v>
       </c>
@@ -6595,7 +6597,7 @@
       </c>
       <c r="D261" s="4"/>
     </row>
-    <row r="262" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A262" s="3">
         <v>6</v>
       </c>
@@ -6607,7 +6609,7 @@
       </c>
       <c r="D262" s="4"/>
     </row>
-    <row r="263" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A263" s="3">
         <v>6</v>
       </c>
@@ -6619,7 +6621,7 @@
       </c>
       <c r="D263" s="4"/>
     </row>
-    <row r="264" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A264" s="3">
         <v>6</v>
       </c>
@@ -6631,7 +6633,7 @@
       </c>
       <c r="D264" s="4"/>
     </row>
-    <row r="265" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A265" s="3">
         <v>6</v>
       </c>
@@ -6643,7 +6645,7 @@
       </c>
       <c r="D265" s="4"/>
     </row>
-    <row r="266" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="266" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A266" s="3">
         <v>6</v>
       </c>
@@ -6655,7 +6657,7 @@
       </c>
       <c r="D266" s="4"/>
     </row>
-    <row r="267" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="267" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A267" s="3">
         <v>6</v>
       </c>
@@ -6667,7 +6669,7 @@
       </c>
       <c r="D267" s="4"/>
     </row>
-    <row r="268" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="268" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A268" s="3">
         <v>6</v>
       </c>
@@ -6679,7 +6681,7 @@
       </c>
       <c r="D268" s="4"/>
     </row>
-    <row r="269" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A269" s="3">
         <v>6</v>
       </c>
@@ -6691,7 +6693,7 @@
       </c>
       <c r="D269" s="4"/>
     </row>
-    <row r="270" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A270" s="3">
         <v>6</v>
       </c>
@@ -6703,7 +6705,7 @@
       </c>
       <c r="D270" s="4"/>
     </row>
-    <row r="271" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="271" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A271" s="3">
         <v>6</v>
       </c>
@@ -6715,7 +6717,7 @@
       </c>
       <c r="D271" s="4"/>
     </row>
-    <row r="272" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="272" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A272" s="3">
         <v>6</v>
       </c>
@@ -6727,7 +6729,7 @@
       </c>
       <c r="D272" s="4"/>
     </row>
-    <row r="273" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A273" s="3">
         <v>6</v>
       </c>
@@ -6739,7 +6741,7 @@
       </c>
       <c r="D273" s="4"/>
     </row>
-    <row r="274" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A274" s="3">
         <v>6</v>
       </c>
@@ -6751,7 +6753,7 @@
       </c>
       <c r="D274" s="4"/>
     </row>
-    <row r="275" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A275" s="3">
         <v>6</v>
       </c>
@@ -6763,7 +6765,7 @@
       </c>
       <c r="D275" s="4"/>
     </row>
-    <row r="276" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A276" s="3">
         <v>6</v>
       </c>
@@ -6775,7 +6777,7 @@
       </c>
       <c r="D276" s="4"/>
     </row>
-    <row r="277" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A277" s="3">
         <v>6</v>
       </c>
@@ -6787,7 +6789,7 @@
       </c>
       <c r="D277" s="4"/>
     </row>
-    <row r="278" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A278" s="3">
         <v>7</v>
       </c>
@@ -6799,7 +6801,7 @@
       </c>
       <c r="D278" s="4"/>
     </row>
-    <row r="279" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A279" s="3">
         <v>7</v>
       </c>
@@ -6811,7 +6813,7 @@
       </c>
       <c r="D279" s="4"/>
     </row>
-    <row r="280" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="280" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A280" s="3">
         <v>7</v>
       </c>
@@ -6823,7 +6825,7 @@
       </c>
       <c r="D280" s="4"/>
     </row>
-    <row r="281" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A281" s="3">
         <v>7</v>
       </c>
@@ -6835,7 +6837,7 @@
       </c>
       <c r="D281" s="4"/>
     </row>
-    <row r="282" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A282" s="3">
         <v>7</v>
       </c>
@@ -6847,7 +6849,7 @@
       </c>
       <c r="D282" s="4"/>
     </row>
-    <row r="283" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A283" s="3">
         <v>7</v>
       </c>
@@ -6859,7 +6861,7 @@
       </c>
       <c r="D283" s="4"/>
     </row>
-    <row r="284" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A284" s="3">
         <v>7</v>
       </c>
@@ -6871,7 +6873,7 @@
       </c>
       <c r="D284" s="4"/>
     </row>
-    <row r="285" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A285" s="3">
         <v>7</v>
       </c>
@@ -6883,7 +6885,7 @@
       </c>
       <c r="D285" s="4"/>
     </row>
-    <row r="286" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A286" s="3">
         <v>7</v>
       </c>
@@ -6895,7 +6897,7 @@
       </c>
       <c r="D286" s="4"/>
     </row>
-    <row r="287" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A287" s="3">
         <v>7</v>
       </c>
@@ -6907,7 +6909,7 @@
       </c>
       <c r="D287" s="4"/>
     </row>
-    <row r="288" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A288" s="3">
         <v>7</v>
       </c>
@@ -6919,7 +6921,7 @@
       </c>
       <c r="D288" s="4"/>
     </row>
-    <row r="289" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="289" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A289" s="3">
         <v>7</v>
       </c>
@@ -6931,7 +6933,7 @@
       </c>
       <c r="D289" s="4"/>
     </row>
-    <row r="290" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="290" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A290" s="3">
         <v>7</v>
       </c>
@@ -6943,7 +6945,7 @@
       </c>
       <c r="D290" s="4"/>
     </row>
-    <row r="291" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="291" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A291" s="3">
         <v>7</v>
       </c>
@@ -6955,7 +6957,7 @@
       </c>
       <c r="D291" s="4"/>
     </row>
-    <row r="292" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="292" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A292" s="3">
         <v>7</v>
       </c>
@@ -6967,7 +6969,7 @@
       </c>
       <c r="D292" s="4"/>
     </row>
-    <row r="293" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="293" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A293" s="3">
         <v>7</v>
       </c>
@@ -6979,7 +6981,7 @@
       </c>
       <c r="D293" s="4"/>
     </row>
-    <row r="294" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="294" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A294" s="3">
         <v>7</v>
       </c>
@@ -6991,7 +6993,7 @@
       </c>
       <c r="D294" s="4"/>
     </row>
-    <row r="295" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="295" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A295" s="3">
         <v>7</v>
       </c>
@@ -7003,7 +7005,7 @@
       </c>
       <c r="D295" s="4"/>
     </row>
-    <row r="296" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="296" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A296" s="3">
         <v>7</v>
       </c>
@@ -7015,7 +7017,7 @@
       </c>
       <c r="D296" s="4"/>
     </row>
-    <row r="297" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="297" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A297" s="3">
         <v>7</v>
       </c>
@@ -7027,7 +7029,7 @@
       </c>
       <c r="D297" s="4"/>
     </row>
-    <row r="298" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="298" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A298" s="3">
         <v>7</v>
       </c>
@@ -7039,7 +7041,7 @@
       </c>
       <c r="D298" s="4"/>
     </row>
-    <row r="299" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="299" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A299" s="3">
         <v>7</v>
       </c>
@@ -7051,7 +7053,7 @@
       </c>
       <c r="D299" s="4"/>
     </row>
-    <row r="300" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="300" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A300" s="3">
         <v>7</v>
       </c>
@@ -7063,7 +7065,7 @@
       </c>
       <c r="D300" s="4"/>
     </row>
-    <row r="301" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="301" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A301" s="3">
         <v>7</v>
       </c>
@@ -7075,7 +7077,7 @@
       </c>
       <c r="D301" s="4"/>
     </row>
-    <row r="302" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="302" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A302" s="3">
         <v>7</v>
       </c>
@@ -7087,7 +7089,7 @@
       </c>
       <c r="D302" s="4"/>
     </row>
-    <row r="303" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A303" s="3">
         <v>7</v>
       </c>
@@ -7099,7 +7101,7 @@
       </c>
       <c r="D303" s="4"/>
     </row>
-    <row r="304" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="304" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A304" s="3">
         <v>7</v>
       </c>
@@ -7111,7 +7113,7 @@
       </c>
       <c r="D304" s="4"/>
     </row>
-    <row r="305" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="305" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A305" s="3">
         <v>7</v>
       </c>
@@ -7123,7 +7125,7 @@
       </c>
       <c r="D305" s="4"/>
     </row>
-    <row r="306" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="306" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A306" s="3">
         <v>7</v>
       </c>
@@ -7135,7 +7137,7 @@
       </c>
       <c r="D306" s="4"/>
     </row>
-    <row r="307" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="307" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A307" s="3">
         <v>7</v>
       </c>
@@ -7147,7 +7149,7 @@
       </c>
       <c r="D307" s="4"/>
     </row>
-    <row r="308" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="308" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A308" s="3">
         <v>7</v>
       </c>
@@ -7159,7 +7161,7 @@
       </c>
       <c r="D308" s="4"/>
     </row>
-    <row r="309" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="309" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A309" s="3">
         <v>7</v>
       </c>
@@ -7171,7 +7173,7 @@
       </c>
       <c r="D309" s="4"/>
     </row>
-    <row r="310" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="310" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A310" s="3">
         <v>7</v>
       </c>
@@ -7183,7 +7185,7 @@
       </c>
       <c r="D310" s="4"/>
     </row>
-    <row r="311" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="311" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A311" s="3">
         <v>7</v>
       </c>
@@ -7195,7 +7197,7 @@
       </c>
       <c r="D311" s="4"/>
     </row>
-    <row r="312" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="312" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A312" s="3">
         <v>7</v>
       </c>
@@ -7207,7 +7209,7 @@
       </c>
       <c r="D312" s="4"/>
     </row>
-    <row r="313" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="313" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A313" s="3">
         <v>7</v>
       </c>
@@ -7219,7 +7221,7 @@
       </c>
       <c r="D313" s="4"/>
     </row>
-    <row r="314" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="314" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A314" s="3">
         <v>7</v>
       </c>
@@ -7231,7 +7233,7 @@
       </c>
       <c r="D314" s="4"/>
     </row>
-    <row r="315" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="315" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A315" s="3">
         <v>7</v>
       </c>
@@ -7243,7 +7245,7 @@
       </c>
       <c r="D315" s="4"/>
     </row>
-    <row r="316" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="316" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A316" s="3">
         <v>7</v>
       </c>
@@ -7255,7 +7257,7 @@
       </c>
       <c r="D316" s="4"/>
     </row>
-    <row r="317" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="317" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A317" s="3">
         <v>9</v>
       </c>
@@ -7267,7 +7269,7 @@
       </c>
       <c r="D317" s="4"/>
     </row>
-    <row r="318" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="318" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A318" s="3">
         <v>9</v>
       </c>
@@ -7279,7 +7281,7 @@
       </c>
       <c r="D318" s="4"/>
     </row>
-    <row r="319" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="319" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A319" s="3">
         <v>9</v>
       </c>
@@ -7291,7 +7293,7 @@
       </c>
       <c r="D319" s="4"/>
     </row>
-    <row r="320" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="320" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A320" s="3">
         <v>9</v>
       </c>
@@ -7303,7 +7305,7 @@
       </c>
       <c r="D320" s="4"/>
     </row>
-    <row r="321" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="321" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A321" s="3">
         <v>9</v>
       </c>
@@ -7315,7 +7317,7 @@
       </c>
       <c r="D321" s="4"/>
     </row>
-    <row r="322" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="322" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A322" s="3">
         <v>9</v>
       </c>
@@ -7327,7 +7329,7 @@
       </c>
       <c r="D322" s="4"/>
     </row>
-    <row r="323" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="323" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A323" s="3">
         <v>9</v>
       </c>
@@ -7339,7 +7341,7 @@
       </c>
       <c r="D323" s="4"/>
     </row>
-    <row r="324" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="324" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A324" s="3">
         <v>9</v>
       </c>
@@ -7351,7 +7353,7 @@
       </c>
       <c r="D324" s="4"/>
     </row>
-    <row r="325" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="325" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A325" s="3">
         <v>9</v>
       </c>
@@ -7363,7 +7365,7 @@
       </c>
       <c r="D325" s="4"/>
     </row>
-    <row r="326" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="326" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A326" s="3">
         <v>9</v>
       </c>
@@ -7375,7 +7377,7 @@
       </c>
       <c r="D326" s="4"/>
     </row>
-    <row r="327" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="327" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A327" s="3">
         <v>9</v>
       </c>
@@ -7387,7 +7389,7 @@
       </c>
       <c r="D327" s="4"/>
     </row>
-    <row r="328" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="328" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A328" s="3">
         <v>9</v>
       </c>
@@ -7399,7 +7401,7 @@
       </c>
       <c r="D328" s="4"/>
     </row>
-    <row r="329" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="329" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A329" s="3">
         <v>9</v>
       </c>
@@ -7411,7 +7413,7 @@
       </c>
       <c r="D329" s="4"/>
     </row>
-    <row r="330" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="330" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A330" s="3">
         <v>9</v>
       </c>
@@ -7423,7 +7425,7 @@
       </c>
       <c r="D330" s="4"/>
     </row>
-    <row r="331" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="331" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A331" s="3">
         <v>9</v>
       </c>
@@ -7435,7 +7437,7 @@
       </c>
       <c r="D331" s="4"/>
     </row>
-    <row r="332" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="332" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A332" s="3">
         <v>9</v>
       </c>
@@ -7447,7 +7449,7 @@
       </c>
       <c r="D332" s="4"/>
     </row>
-    <row r="333" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="333" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A333" s="3">
         <v>9</v>
       </c>
@@ -7459,7 +7461,7 @@
       </c>
       <c r="D333" s="4"/>
     </row>
-    <row r="334" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="334" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A334" s="3">
         <v>9</v>
       </c>
@@ -7471,7 +7473,7 @@
       </c>
       <c r="D334" s="4"/>
     </row>
-    <row r="335" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="335" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A335" s="3">
         <v>9</v>
       </c>
@@ -7483,7 +7485,7 @@
       </c>
       <c r="D335" s="4"/>
     </row>
-    <row r="336" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="336" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A336" s="3">
         <v>9</v>
       </c>
@@ -7495,7 +7497,7 @@
       </c>
       <c r="D336" s="4"/>
     </row>
-    <row r="337" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="337" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A337" s="3">
         <v>9</v>
       </c>
@@ -7507,7 +7509,7 @@
       </c>
       <c r="D337" s="4"/>
     </row>
-    <row r="338" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="338" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A338" s="3">
         <v>9</v>
       </c>
@@ -7519,7 +7521,7 @@
       </c>
       <c r="D338" s="4"/>
     </row>
-    <row r="339" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="339" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A339" s="3">
         <v>9</v>
       </c>
@@ -7531,7 +7533,7 @@
       </c>
       <c r="D339" s="4"/>
     </row>
-    <row r="340" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="340" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A340" s="3">
         <v>9</v>
       </c>
@@ -7543,7 +7545,7 @@
       </c>
       <c r="D340" s="4"/>
     </row>
-    <row r="341" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="341" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A341" s="3">
         <v>9</v>
       </c>
@@ -7555,7 +7557,7 @@
       </c>
       <c r="D341" s="4"/>
     </row>
-    <row r="342" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="342" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A342" s="3">
         <v>9</v>
       </c>
@@ -7567,7 +7569,7 @@
       </c>
       <c r="D342" s="4"/>
     </row>
-    <row r="343" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="343" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A343" s="3">
         <v>9</v>
       </c>
@@ -7579,7 +7581,7 @@
       </c>
       <c r="D343" s="4"/>
     </row>
-    <row r="344" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="344" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A344" s="3">
         <v>9</v>
       </c>
@@ -7591,7 +7593,7 @@
       </c>
       <c r="D344" s="4"/>
     </row>
-    <row r="345" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="345" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A345" s="3">
         <v>9</v>
       </c>
@@ -7603,7 +7605,7 @@
       </c>
       <c r="D345" s="4"/>
     </row>
-    <row r="346" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="346" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A346" s="3">
         <v>9</v>
       </c>
@@ -7615,7 +7617,7 @@
       </c>
       <c r="D346" s="4"/>
     </row>
-    <row r="347" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="347" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A347" s="3">
         <v>9</v>
       </c>
@@ -7627,7 +7629,7 @@
       </c>
       <c r="D347" s="4"/>
     </row>
-    <row r="348" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="348" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A348" s="3">
         <v>9</v>
       </c>
@@ -7639,7 +7641,7 @@
       </c>
       <c r="D348" s="4"/>
     </row>
-    <row r="349" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="349" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A349" s="3">
         <v>9</v>
       </c>
@@ -7651,7 +7653,7 @@
       </c>
       <c r="D349" s="4"/>
     </row>
-    <row r="350" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="350" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A350" s="3">
         <v>9</v>
       </c>
@@ -7663,7 +7665,7 @@
       </c>
       <c r="D350" s="4"/>
     </row>
-    <row r="351" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="351" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A351" s="3">
         <v>9</v>
       </c>
@@ -7675,7 +7677,7 @@
       </c>
       <c r="D351" s="4"/>
     </row>
-    <row r="352" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="352" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A352" s="3">
         <v>9</v>
       </c>
@@ -7687,7 +7689,7 @@
       </c>
       <c r="D352" s="4"/>
     </row>
-    <row r="353" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="353" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A353" s="3">
         <v>9</v>
       </c>
@@ -7699,7 +7701,7 @@
       </c>
       <c r="D353" s="4"/>
     </row>
-    <row r="354" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="354" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A354" s="3">
         <v>9</v>
       </c>
@@ -7711,7 +7713,7 @@
       </c>
       <c r="D354" s="4"/>
     </row>
-    <row r="355" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="355" spans="1:4" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
       <c r="A355" s="3">
         <v>9</v>
       </c>
@@ -8581,7 +8583,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="434" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A434" s="2">
         <v>12</v>
       </c>
@@ -8592,7 +8594,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="435" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A435" s="2">
         <v>12</v>
       </c>
@@ -8603,7 +8605,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="436" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A436" s="2">
         <v>12</v>
       </c>
@@ -8614,7 +8616,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="437" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A437" s="2">
         <v>12</v>
       </c>
@@ -8625,7 +8627,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="438" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A438" s="2">
         <v>12</v>
       </c>
@@ -8636,7 +8638,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="439" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A439" s="2">
         <v>12</v>
       </c>
@@ -8647,7 +8649,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="440" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A440" s="2">
         <v>12</v>
       </c>
@@ -8658,7 +8660,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="441" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A441" s="2">
         <v>12</v>
       </c>
@@ -8669,7 +8671,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="442" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A442" s="2">
         <v>12</v>
       </c>
@@ -8680,7 +8682,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="443" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A443" s="2">
         <v>12</v>
       </c>
@@ -8691,7 +8693,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="444" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A444" s="2">
         <v>12</v>
       </c>
@@ -8702,7 +8704,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="445" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A445" s="2">
         <v>12</v>
       </c>
@@ -8713,7 +8715,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="446" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A446" s="2">
         <v>12</v>
       </c>
@@ -8724,7 +8726,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="447" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A447" s="2">
         <v>12</v>
       </c>
@@ -8735,7 +8737,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="448" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A448" s="2">
         <v>12</v>
       </c>
@@ -8746,7 +8748,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="449" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A449" s="2">
         <v>12</v>
       </c>
@@ -8757,7 +8759,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="450" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A450" s="2">
         <v>12</v>
       </c>
@@ -8768,7 +8770,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="451" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A451" s="2">
         <v>12</v>
       </c>
@@ -8779,7 +8781,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="452" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A452" s="2">
         <v>12</v>
       </c>
@@ -8790,7 +8792,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="453" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A453" s="2">
         <v>12</v>
       </c>
@@ -8801,7 +8803,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="454" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A454" s="2">
         <v>12</v>
       </c>
@@ -8812,7 +8814,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="455" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="455" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A455" s="2">
         <v>12</v>
       </c>
@@ -8823,7 +8825,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="456" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A456" s="2">
         <v>12</v>
       </c>
@@ -8834,7 +8836,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="457" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="457" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A457" s="2">
         <v>12</v>
       </c>
@@ -8845,7 +8847,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="458" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="458" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A458" s="2">
         <v>12</v>
       </c>
@@ -8856,7 +8858,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="459" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A459" s="2">
         <v>12</v>
       </c>
@@ -8867,7 +8869,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="460" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A460" s="2">
         <v>12</v>
       </c>
@@ -8878,7 +8880,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="461" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="461" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A461" s="2">
         <v>12</v>
       </c>
@@ -8889,7 +8891,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="462" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A462" s="2">
         <v>12</v>
       </c>
@@ -8900,7 +8902,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="463" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A463" s="2">
         <v>12</v>
       </c>
@@ -8911,7 +8913,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="464" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A464" s="2">
         <v>12</v>
       </c>
@@ -8922,7 +8924,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="465" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A465" s="2">
         <v>12</v>
       </c>
@@ -8933,7 +8935,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="466" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A466" s="2">
         <v>12</v>
       </c>
@@ -8944,7 +8946,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="467" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A467" s="2">
         <v>12</v>
       </c>
@@ -8955,7 +8957,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="468" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="468" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A468" s="2">
         <v>12</v>
       </c>
@@ -8966,7 +8968,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="469" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A469" s="2">
         <v>12</v>
       </c>
@@ -8977,7 +8979,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="470" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="470" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A470" s="2">
         <v>12</v>
       </c>
@@ -8988,7 +8990,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="471" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="471" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A471" s="2">
         <v>12</v>
       </c>
@@ -8999,7 +9001,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="472" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="472" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A472" s="2">
         <v>12</v>
       </c>
@@ -9010,7 +9012,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="473" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="473" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A473" s="2">
         <v>13</v>
       </c>
@@ -9021,7 +9023,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="474" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="474" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A474" s="2">
         <v>13</v>
       </c>
@@ -9032,7 +9034,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="475" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="475" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A475" s="2">
         <v>13</v>
       </c>
@@ -9043,7 +9045,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="476" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="476" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A476" s="2">
         <v>13</v>
       </c>
@@ -9054,7 +9056,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="477" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="477" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A477" s="2">
         <v>13</v>
       </c>
@@ -9065,7 +9067,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="478" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="478" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A478" s="2">
         <v>13</v>
       </c>
@@ -9076,7 +9078,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="479" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="479" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A479" s="2">
         <v>13</v>
       </c>
@@ -9087,7 +9089,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="480" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A480" s="2">
         <v>13</v>
       </c>
@@ -9098,7 +9100,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="481" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A481" s="2">
         <v>13</v>
       </c>
@@ -9109,7 +9111,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="482" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="482" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A482" s="2">
         <v>13</v>
       </c>
@@ -9120,7 +9122,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="483" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A483" s="2">
         <v>13</v>
       </c>
@@ -9131,7 +9133,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="484" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A484" s="2">
         <v>13</v>
       </c>
@@ -9142,7 +9144,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="485" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A485" s="2">
         <v>13</v>
       </c>
@@ -9153,7 +9155,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="486" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A486" s="2">
         <v>13</v>
       </c>
@@ -9164,7 +9166,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="487" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A487" s="2">
         <v>13</v>
       </c>
@@ -9175,7 +9177,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="488" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A488" s="2">
         <v>13</v>
       </c>
@@ -9186,7 +9188,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="489" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A489" s="2">
         <v>13</v>
       </c>
@@ -9197,7 +9199,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="490" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A490" s="2">
         <v>13</v>
       </c>
@@ -9208,7 +9210,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="491" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A491" s="2">
         <v>13</v>
       </c>
@@ -9219,7 +9221,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="492" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="492" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A492" s="2">
         <v>13</v>
       </c>
@@ -9230,7 +9232,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="493" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A493" s="2">
         <v>13</v>
       </c>
@@ -9241,7 +9243,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="494" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A494" s="2">
         <v>13</v>
       </c>
@@ -9252,7 +9254,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="495" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="495" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A495" s="2">
         <v>13</v>
       </c>
@@ -9263,7 +9265,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="496" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="496" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A496" s="2">
         <v>13</v>
       </c>
@@ -9274,7 +9276,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="497" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A497" s="2">
         <v>13</v>
       </c>
@@ -9285,7 +9287,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="498" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="498" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A498" s="2">
         <v>13</v>
       </c>
@@ -9296,7 +9298,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="499" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="499" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A499" s="2">
         <v>13</v>
       </c>
@@ -9307,7 +9309,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="500" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="500" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A500" s="2">
         <v>13</v>
       </c>
@@ -9318,7 +9320,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="501" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="501" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A501" s="2">
         <v>13</v>
       </c>
@@ -9329,7 +9331,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="502" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="502" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A502" s="2">
         <v>13</v>
       </c>
@@ -9340,7 +9342,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="503" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="503" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A503" s="2">
         <v>13</v>
       </c>
@@ -9351,7 +9353,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="504" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="504" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A504" s="2">
         <v>13</v>
       </c>
@@ -9362,7 +9364,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="505" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="505" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A505" s="2">
         <v>13</v>
       </c>
@@ -9373,7 +9375,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="506" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="506" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A506" s="2">
         <v>13</v>
       </c>
@@ -9384,7 +9386,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="507" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="507" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A507" s="2">
         <v>13</v>
       </c>
@@ -9395,7 +9397,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="508" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="508" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A508" s="2">
         <v>13</v>
       </c>
@@ -9406,7 +9408,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="509" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="509" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A509" s="2">
         <v>13</v>
       </c>
@@ -9417,7 +9419,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="510" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="510" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A510" s="2">
         <v>13</v>
       </c>
@@ -9428,7 +9430,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="511" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="511" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A511" s="2">
         <v>13</v>
       </c>
@@ -9439,7 +9441,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="512" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="512" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A512" s="2">
         <v>14</v>
       </c>
@@ -9450,7 +9452,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="513" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="513" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A513" s="2">
         <v>14</v>
       </c>
@@ -9461,7 +9463,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="514" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="514" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A514" s="2">
         <v>14</v>
       </c>
@@ -9472,7 +9474,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="515" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="515" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A515" s="2">
         <v>14</v>
       </c>
@@ -9483,7 +9485,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="516" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="516" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A516" s="2">
         <v>14</v>
       </c>
@@ -9494,7 +9496,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="517" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="517" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A517" s="2">
         <v>14</v>
       </c>
@@ -9505,7 +9507,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="518" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="518" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A518" s="2">
         <v>14</v>
       </c>
@@ -9516,7 +9518,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="519" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="519" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A519" s="2">
         <v>14</v>
       </c>
@@ -9527,7 +9529,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="520" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="520" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A520" s="2">
         <v>14</v>
       </c>
@@ -9538,7 +9540,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="521" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="521" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A521" s="2">
         <v>14</v>
       </c>
@@ -9549,7 +9551,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="522" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="522" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A522" s="2">
         <v>14</v>
       </c>
@@ -9560,7 +9562,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="523" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="523" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A523" s="2">
         <v>14</v>
       </c>
@@ -9571,7 +9573,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="524" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="524" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A524" s="2">
         <v>14</v>
       </c>
@@ -9582,7 +9584,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="525" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="525" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A525" s="2">
         <v>14</v>
       </c>
@@ -9593,7 +9595,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="526" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="526" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A526" s="2">
         <v>14</v>
       </c>
@@ -9604,7 +9606,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="527" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="527" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A527" s="2">
         <v>14</v>
       </c>
@@ -9615,7 +9617,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="528" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="528" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A528" s="2">
         <v>14</v>
       </c>
@@ -9626,7 +9628,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="529" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="529" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A529" s="2">
         <v>14</v>
       </c>
@@ -9637,7 +9639,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="530" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="530" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A530" s="2">
         <v>14</v>
       </c>
@@ -9648,7 +9650,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="531" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="531" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A531" s="2">
         <v>14</v>
       </c>
@@ -9659,7 +9661,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="532" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="532" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A532" s="2">
         <v>14</v>
       </c>
@@ -9670,7 +9672,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="533" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="533" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A533" s="2">
         <v>14</v>
       </c>
@@ -9681,7 +9683,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="534" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="534" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A534" s="2">
         <v>14</v>
       </c>
@@ -9692,7 +9694,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="535" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="535" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A535" s="2">
         <v>14</v>
       </c>
@@ -9703,7 +9705,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="536" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="536" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A536" s="2">
         <v>14</v>
       </c>
@@ -9714,7 +9716,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="537" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="537" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A537" s="2">
         <v>14</v>
       </c>
@@ -9725,7 +9727,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="538" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="538" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A538" s="2">
         <v>14</v>
       </c>
@@ -9736,7 +9738,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="539" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="539" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A539" s="2">
         <v>14</v>
       </c>
@@ -9747,7 +9749,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="540" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="540" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A540" s="2">
         <v>14</v>
       </c>
@@ -9758,7 +9760,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="541" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="541" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A541" s="2">
         <v>14</v>
       </c>
@@ -9769,7 +9771,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="542" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="542" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A542" s="2">
         <v>14</v>
       </c>
@@ -9780,7 +9782,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="543" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="543" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A543" s="2">
         <v>14</v>
       </c>
@@ -9791,7 +9793,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="544" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="544" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A544" s="2">
         <v>14</v>
       </c>
@@ -9802,7 +9804,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="545" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="545" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A545" s="2">
         <v>14</v>
       </c>
@@ -9813,7 +9815,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="546" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="546" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A546" s="2">
         <v>14</v>
       </c>
@@ -9824,7 +9826,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="547" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="547" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A547" s="2">
         <v>14</v>
       </c>
@@ -9835,7 +9837,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="548" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="548" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A548" s="2">
         <v>14</v>
       </c>
@@ -9846,7 +9848,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="549" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="549" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A549" s="2">
         <v>14</v>
       </c>
@@ -9857,7 +9859,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="550" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="550" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A550" s="2">
         <v>14</v>
       </c>
@@ -9868,7 +9870,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="551" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="551" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A551" s="2">
         <v>15</v>
       </c>
@@ -9879,7 +9881,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="552" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="552" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A552" s="2">
         <v>15</v>
       </c>
@@ -9890,7 +9892,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="553" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="553" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A553" s="2">
         <v>15</v>
       </c>
@@ -9901,7 +9903,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="554" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="554" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A554" s="2">
         <v>15</v>
       </c>
@@ -9912,7 +9914,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="555" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="555" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A555" s="2">
         <v>15</v>
       </c>
@@ -9923,7 +9925,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="556" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="556" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A556" s="2">
         <v>15</v>
       </c>
@@ -9934,7 +9936,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="557" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="557" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A557" s="2">
         <v>15</v>
       </c>
@@ -9945,7 +9947,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="558" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="558" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A558" s="2">
         <v>15</v>
       </c>
@@ -9956,7 +9958,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="559" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="559" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A559" s="2">
         <v>15</v>
       </c>
@@ -9967,7 +9969,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="560" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="560" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A560" s="2">
         <v>15</v>
       </c>
@@ -9978,7 +9980,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="561" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="561" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A561" s="2">
         <v>15</v>
       </c>
@@ -9989,7 +9991,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="562" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="562" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A562" s="2">
         <v>15</v>
       </c>
@@ -10000,7 +10002,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="563" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="563" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A563" s="2">
         <v>15</v>
       </c>
@@ -10011,7 +10013,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="564" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="564" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A564" s="2">
         <v>15</v>
       </c>
@@ -10022,7 +10024,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="565" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="565" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A565" s="2">
         <v>15</v>
       </c>
@@ -10033,7 +10035,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="566" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="566" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A566" s="2">
         <v>15</v>
       </c>
@@ -10044,7 +10046,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="567" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="567" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A567" s="2">
         <v>15</v>
       </c>
@@ -10055,7 +10057,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="568" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="568" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A568" s="2">
         <v>15</v>
       </c>
@@ -10066,7 +10068,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="569" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="569" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A569" s="2">
         <v>15</v>
       </c>
@@ -10077,7 +10079,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="570" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="570" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A570" s="2">
         <v>15</v>
       </c>
@@ -10088,7 +10090,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="571" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="571" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A571" s="2">
         <v>15</v>
       </c>
@@ -10099,7 +10101,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="572" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="572" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A572" s="2">
         <v>15</v>
       </c>
@@ -10110,7 +10112,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="573" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="573" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A573" s="2">
         <v>15</v>
       </c>
@@ -10121,7 +10123,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="574" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="574" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A574" s="2">
         <v>15</v>
       </c>
@@ -10132,7 +10134,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="575" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="575" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A575" s="2">
         <v>15</v>
       </c>
@@ -10143,7 +10145,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="576" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="576" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A576" s="2">
         <v>15</v>
       </c>
@@ -10154,7 +10156,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="577" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="577" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A577" s="2">
         <v>15</v>
       </c>
@@ -10165,7 +10167,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="578" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="578" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A578" s="2">
         <v>15</v>
       </c>
@@ -10176,7 +10178,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="579" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="579" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A579" s="2">
         <v>15</v>
       </c>
@@ -10187,7 +10189,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="580" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="580" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A580" s="2">
         <v>15</v>
       </c>
@@ -10198,7 +10200,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="581" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="581" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A581" s="2">
         <v>15</v>
       </c>
@@ -10209,7 +10211,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="582" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="582" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A582" s="2">
         <v>15</v>
       </c>
@@ -10220,7 +10222,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="583" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="583" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A583" s="2">
         <v>15</v>
       </c>
@@ -10231,7 +10233,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="584" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="584" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A584" s="2">
         <v>15</v>
       </c>
@@ -10242,7 +10244,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="585" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="585" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A585" s="2">
         <v>15</v>
       </c>
@@ -10253,7 +10255,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="586" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="586" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A586" s="2">
         <v>15</v>
       </c>
@@ -10264,7 +10266,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="587" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="587" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A587" s="2">
         <v>15</v>
       </c>
@@ -10275,7 +10277,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="588" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="588" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A588" s="2">
         <v>15</v>
       </c>
@@ -10286,7 +10288,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="589" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="589" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A589" s="2">
         <v>15</v>
       </c>
@@ -10298,6 +10300,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A589">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="10"/>
+        <filter val="11"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>